<commit_message>
update for simple tables in the guidebook
</commit_message>
<xml_diff>
--- a/Analysis/figTbl_guidebook/experiment_detMeasures(4).xlsx
+++ b/Analysis/figTbl_guidebook/experiment_detMeasures(4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim_riskSharing\Analysis\figTbl_guidebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC31449-754B-41B6-A425-67620E2E6DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8133353C-B058-4A06-90E8-22FF7FB1D4E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="detMeasures" sheetId="1" r:id="rId1"/>
@@ -907,6 +907,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,12 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4527,10 +4527,10 @@
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="130"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="36"/>
       <c r="F6" s="37" t="s">
         <v>52</v>
@@ -5036,17 +5036,17 @@
     <row r="6" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
       <c r="B6" s="43"/>
-      <c r="C6" s="131" t="s">
+      <c r="C6" s="133" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="132" t="s">
+      <c r="G6" s="134" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
       <c r="J6" s="29"/>
     </row>
     <row r="7" spans="1:13" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5434,8 +5434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AC6BED-6E6B-43AC-B690-CD2222CF03DF}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7529,29 +7529,29 @@
     <row r="20" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="43"/>
-      <c r="C20" s="133" t="s">
+      <c r="C20" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="133"/>
-      <c r="E20" s="133"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="103"/>
-      <c r="G20" s="133" t="s">
+      <c r="G20" s="135" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
       <c r="J20" s="103"/>
-      <c r="K20" s="133" t="s">
+      <c r="K20" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="133"/>
-      <c r="M20" s="133"/>
+      <c r="L20" s="135"/>
+      <c r="M20" s="135"/>
       <c r="N20" s="43"/>
-      <c r="O20" s="133" t="s">
+      <c r="O20" s="135" t="s">
         <v>101</v>
       </c>
-      <c r="P20" s="133"/>
-      <c r="Q20" s="133"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="135"/>
       <c r="R20" s="29"/>
     </row>
     <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -8476,8 +8476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BDDED7-C10A-4804-B5B6-56434A54CAA8}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8694,23 +8694,23 @@
     <row r="12" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="43"/>
-      <c r="C12" s="133" t="s">
+      <c r="C12" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="103"/>
-      <c r="G12" s="133" t="s">
+      <c r="G12" s="135" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
       <c r="J12" s="103"/>
-      <c r="K12" s="133" t="s">
+      <c r="K12" s="135" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
       <c r="N12" s="29"/>
     </row>
     <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -8719,7 +8719,7 @@
       <c r="C13" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="130" t="s">
         <v>102</v>
       </c>
       <c r="E13" s="112" t="s">
@@ -8729,7 +8729,7 @@
       <c r="G13" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="134" t="s">
+      <c r="H13" s="130" t="s">
         <v>102</v>
       </c>
       <c r="I13" s="112" t="s">
@@ -8739,7 +8739,7 @@
       <c r="K13" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="134" t="s">
+      <c r="L13" s="130" t="s">
         <v>102</v>
       </c>
       <c r="M13" s="112" t="s">
@@ -8749,7 +8749,7 @@
     </row>
     <row r="14" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
-      <c r="B14" s="135" t="s">
+      <c r="B14" s="131" t="s">
         <v>118</v>
       </c>
       <c r="C14" s="103"/>
@@ -8810,7 +8810,7 @@
       </c>
       <c r="N15" s="43"/>
     </row>
-    <row r="16" spans="1:14" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="128" t="s">
         <v>117</v>

</xml_diff>